<commit_message>
VCF-SV: don't have to buy a hole
</commit_message>
<xml_diff>
--- a/modules/VCF-SV/VCF-SV-BOM.xlsx
+++ b/modules/VCF-SV/VCF-SV-BOM.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\VCF-SV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4247AB13-13A1-4116-A839-E7DDC850F9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEC56DB-6DB1-46F6-A10E-4E13D31A96CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="2190" windowWidth="19380" windowHeight="11820"/>
+    <workbookView xWindow="5655" yWindow="1545" windowWidth="19380" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VCF-SV-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="290">
   <si>
     <t>Ref</t>
   </si>
@@ -326,12 +339,6 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/3525</t>
-  </si>
-  <si>
-    <t>H12 H13</t>
-  </si>
-  <si>
-    <t>WireHole_PTH</t>
   </si>
   <si>
     <t>J1 J2 J3 J4 J5 J6</t>
@@ -901,7 +908,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1747,11 +1754,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,13 +1775,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1872,7 +1879,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E40" si="0">MAX(B3-C3-D3,0)</f>
+        <f t="shared" ref="E3:E39" si="0">MAX(B3-C3-D3,0)</f>
         <v>2</v>
       </c>
       <c r="F3" t="s">
@@ -2220,73 +2227,94 @@
         <v>102</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F12" t="s">
         <v>103</v>
       </c>
+      <c r="I12" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" t="s">
+        <v>105</v>
+      </c>
+      <c r="K12" t="s">
+        <v>106</v>
+      </c>
+      <c r="L12" t="s">
+        <v>107</v>
+      </c>
+      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" t="s">
+        <v>108</v>
+      </c>
+      <c r="O12" t="s">
+        <v>109</v>
+      </c>
+      <c r="P12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>110</v>
+      </c>
+      <c r="R12" t="s">
+        <v>111</v>
+      </c>
+      <c r="S12" t="s">
+        <v>100</v>
+      </c>
+      <c r="T12">
+        <v>4031</v>
+      </c>
+      <c r="U12" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="I13" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="J13" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="K13" t="s">
-        <v>108</v>
-      </c>
-      <c r="L13" t="s">
-        <v>109</v>
+        <v>117</v>
+      </c>
+      <c r="L13">
+        <v>61201621621</v>
       </c>
       <c r="M13" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="N13" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="O13" t="s">
-        <v>111</v>
-      </c>
-      <c r="P13" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>112</v>
-      </c>
-      <c r="R13" t="s">
-        <v>113</v>
-      </c>
-      <c r="S13" t="s">
-        <v>100</v>
-      </c>
-      <c r="T13">
-        <v>4031</v>
-      </c>
-      <c r="U13" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2296,69 +2324,69 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="I14" t="s">
-        <v>117</v>
-      </c>
-      <c r="J14" t="s">
-        <v>118</v>
-      </c>
-      <c r="K14" t="s">
-        <v>119</v>
-      </c>
-      <c r="L14">
-        <v>61201621621</v>
+        <v>122</v>
       </c>
       <c r="M14" t="s">
+        <v>100</v>
+      </c>
+      <c r="N14">
+        <v>598</v>
+      </c>
+      <c r="O14" t="s">
+        <v>123</v>
+      </c>
+      <c r="P14" t="s">
         <v>36</v>
       </c>
-      <c r="N14" t="s">
-        <v>120</v>
-      </c>
-      <c r="O14" t="s">
-        <v>121</v>
+      <c r="Q14" t="s">
+        <v>124</v>
+      </c>
+      <c r="R14" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>127</v>
+      </c>
+      <c r="I15" t="s">
         <v>122</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>123</v>
-      </c>
-      <c r="I15" t="s">
-        <v>124</v>
       </c>
       <c r="M15" t="s">
         <v>100</v>
       </c>
       <c r="N15">
-        <v>598</v>
+        <v>392</v>
       </c>
       <c r="O15" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="P15" t="s">
         <v>36</v>
       </c>
       <c r="Q15" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="R15" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2368,10 +2396,10 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I16" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="M16" t="s">
         <v>100</v>
@@ -2380,21 +2408,21 @@
         <v>392</v>
       </c>
       <c r="O16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P16" t="s">
         <v>36</v>
       </c>
       <c r="Q16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="R16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2404,150 +2432,153 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+      <c r="G17" t="s">
+        <v>136</v>
       </c>
       <c r="I17" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="J17" t="s">
+        <v>138</v>
+      </c>
+      <c r="K17" t="s">
+        <v>139</v>
+      </c>
+      <c r="L17" t="s">
+        <v>140</v>
       </c>
       <c r="M17" t="s">
-        <v>100</v>
-      </c>
-      <c r="N17">
-        <v>392</v>
+        <v>36</v>
+      </c>
+      <c r="N17" t="s">
+        <v>141</v>
       </c>
       <c r="O17" t="s">
-        <v>130</v>
-      </c>
-      <c r="P17" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>131</v>
-      </c>
-      <c r="R17" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>144</v>
+      </c>
+      <c r="G18" t="s">
         <v>136</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="I18" t="s">
         <v>137</v>
       </c>
-      <c r="G18" t="s">
+      <c r="J18" t="s">
         <v>138</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>139</v>
       </c>
-      <c r="J18" t="s">
-        <v>140</v>
-      </c>
-      <c r="K18" t="s">
-        <v>141</v>
-      </c>
       <c r="L18" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="M18" t="s">
         <v>36</v>
       </c>
       <c r="N18" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="O18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G19" t="s">
+        <v>136</v>
+      </c>
+      <c r="I19" t="s">
+        <v>137</v>
+      </c>
+      <c r="J19" t="s">
         <v>138</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>139</v>
       </c>
-      <c r="J19" t="s">
-        <v>140</v>
-      </c>
-      <c r="K19" t="s">
-        <v>141</v>
-      </c>
       <c r="L19" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="M19" t="s">
         <v>36</v>
       </c>
       <c r="N19" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="O19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B20">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" t="s">
+        <v>137</v>
+      </c>
+      <c r="J20" t="s">
         <v>138</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>139</v>
       </c>
-      <c r="J20" t="s">
-        <v>140</v>
-      </c>
-      <c r="K20" t="s">
-        <v>141</v>
-      </c>
       <c r="L20" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="M20" t="s">
         <v>36</v>
       </c>
       <c r="N20" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="O20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2557,114 +2588,114 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="G21" t="s">
+        <v>136</v>
+      </c>
+      <c r="I21" t="s">
+        <v>137</v>
+      </c>
+      <c r="J21" t="s">
         <v>138</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>139</v>
       </c>
-      <c r="J21" t="s">
-        <v>140</v>
-      </c>
-      <c r="K21" t="s">
-        <v>141</v>
-      </c>
       <c r="L21" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="M21" t="s">
         <v>36</v>
       </c>
       <c r="N21" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="O21" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G22" t="s">
+        <v>136</v>
+      </c>
+      <c r="I22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J22" t="s">
         <v>138</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>139</v>
       </c>
-      <c r="J22" t="s">
-        <v>140</v>
-      </c>
-      <c r="K22" t="s">
-        <v>141</v>
-      </c>
       <c r="L22" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="M22" t="s">
         <v>36</v>
       </c>
       <c r="N22" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="O22" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G23" t="s">
+        <v>136</v>
+      </c>
+      <c r="I23" t="s">
+        <v>137</v>
+      </c>
+      <c r="J23" t="s">
         <v>138</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>139</v>
       </c>
-      <c r="J23" t="s">
-        <v>140</v>
-      </c>
-      <c r="K23" t="s">
-        <v>141</v>
-      </c>
       <c r="L23" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="M23" t="s">
         <v>36</v>
       </c>
       <c r="N23" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="O23" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2674,36 +2705,36 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G24" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24" t="s">
+        <v>137</v>
+      </c>
+      <c r="J24" t="s">
         <v>138</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>139</v>
       </c>
-      <c r="J24" t="s">
-        <v>140</v>
-      </c>
-      <c r="K24" t="s">
-        <v>141</v>
-      </c>
       <c r="L24" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="M24" t="s">
         <v>36</v>
       </c>
       <c r="N24" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="O24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2713,36 +2744,36 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G25" t="s">
+        <v>136</v>
+      </c>
+      <c r="I25" t="s">
+        <v>137</v>
+      </c>
+      <c r="J25" t="s">
         <v>138</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>139</v>
       </c>
-      <c r="J25" t="s">
-        <v>140</v>
-      </c>
-      <c r="K25" t="s">
-        <v>141</v>
-      </c>
       <c r="L25" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="M25" t="s">
         <v>36</v>
       </c>
       <c r="N25" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="O25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2752,36 +2783,36 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G26" t="s">
+        <v>136</v>
+      </c>
+      <c r="I26" t="s">
+        <v>137</v>
+      </c>
+      <c r="J26" t="s">
         <v>138</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>139</v>
       </c>
-      <c r="J26" t="s">
-        <v>140</v>
-      </c>
-      <c r="K26" t="s">
-        <v>141</v>
-      </c>
       <c r="L26" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="M26" t="s">
         <v>36</v>
       </c>
       <c r="N26" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="O26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2791,36 +2822,36 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G27" t="s">
+        <v>136</v>
+      </c>
+      <c r="I27" t="s">
+        <v>137</v>
+      </c>
+      <c r="J27" t="s">
         <v>138</v>
       </c>
-      <c r="I27" t="s">
+      <c r="K27" t="s">
         <v>139</v>
       </c>
-      <c r="J27" t="s">
-        <v>140</v>
-      </c>
-      <c r="K27" t="s">
-        <v>141</v>
-      </c>
       <c r="L27" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="M27" t="s">
         <v>36</v>
       </c>
       <c r="N27" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="O27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2830,36 +2861,36 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="G28" t="s">
+        <v>136</v>
+      </c>
+      <c r="I28" t="s">
+        <v>137</v>
+      </c>
+      <c r="J28" t="s">
         <v>138</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>139</v>
       </c>
-      <c r="J28" t="s">
-        <v>140</v>
-      </c>
-      <c r="K28" t="s">
-        <v>141</v>
-      </c>
       <c r="L28" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="M28" t="s">
         <v>36</v>
       </c>
       <c r="N28" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="O28" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -2869,315 +2900,315 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G29" t="s">
+        <v>136</v>
+      </c>
+      <c r="I29" t="s">
+        <v>137</v>
+      </c>
+      <c r="J29" t="s">
         <v>138</v>
       </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>139</v>
       </c>
-      <c r="J29" t="s">
-        <v>140</v>
-      </c>
-      <c r="K29" t="s">
-        <v>141</v>
-      </c>
       <c r="L29" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="M29" t="s">
         <v>36</v>
       </c>
       <c r="N29" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="O29" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G30" t="s">
-        <v>138</v>
+        <v>205</v>
+      </c>
+      <c r="H30" t="s">
+        <v>206</v>
       </c>
       <c r="I30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J30" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
       <c r="K30" t="s">
-        <v>141</v>
+        <v>208</v>
       </c>
       <c r="L30" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="M30" t="s">
         <v>36</v>
       </c>
       <c r="N30" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="O30" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>205</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F31" t="s">
-        <v>206</v>
-      </c>
       <c r="G31" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="H31" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="I31" t="s">
-        <v>139</v>
+        <v>215</v>
       </c>
       <c r="J31" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="K31" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="L31" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="M31" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="N31" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="O31" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="P31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>206</v>
+        <v>149</v>
       </c>
       <c r="G32" t="s">
-        <v>215</v>
-      </c>
-      <c r="H32" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="I32" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="J32" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="K32" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="L32" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="M32" t="s">
         <v>22</v>
       </c>
       <c r="N32" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="O32" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="P32" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>228</v>
+      </c>
+      <c r="R32" t="s">
+        <v>229</v>
+      </c>
+      <c r="S32" t="s">
+        <v>24</v>
+      </c>
+      <c r="T32" t="s">
+        <v>230</v>
+      </c>
+      <c r="U32" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" t="s">
+        <v>221</v>
+      </c>
+      <c r="I33" t="s">
         <v>222</v>
       </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F33" t="s">
-        <v>151</v>
-      </c>
-      <c r="G33" t="s">
-        <v>223</v>
-      </c>
-      <c r="I33" t="s">
-        <v>224</v>
-      </c>
       <c r="J33" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="K33" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="L33" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="M33" t="s">
+        <v>24</v>
+      </c>
+      <c r="N33" t="s">
+        <v>236</v>
+      </c>
+      <c r="O33" t="s">
+        <v>237</v>
+      </c>
+      <c r="P33" t="s">
         <v>22</v>
       </c>
-      <c r="N33" t="s">
-        <v>228</v>
-      </c>
-      <c r="O33" t="s">
-        <v>229</v>
-      </c>
-      <c r="P33" t="s">
-        <v>36</v>
-      </c>
       <c r="Q33" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="R33" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="S33" t="s">
         <v>24</v>
       </c>
       <c r="T33" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="U33" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>151</v>
-      </c>
-      <c r="G34" t="s">
-        <v>223</v>
+        <v>241</v>
+      </c>
+      <c r="H34" t="s">
+        <v>242</v>
       </c>
       <c r="I34" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="J34" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="K34" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="L34" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="M34" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="N34" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="O34" t="s">
-        <v>239</v>
-      </c>
-      <c r="P34" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>240</v>
-      </c>
-      <c r="R34" t="s">
-        <v>241</v>
-      </c>
-      <c r="S34" t="s">
-        <v>24</v>
-      </c>
-      <c r="T34" t="s">
-        <v>232</v>
-      </c>
-      <c r="U34" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>249</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>250</v>
+      </c>
+      <c r="H35" t="s">
         <v>242</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="I35" t="s">
         <v>243</v>
       </c>
-      <c r="H35" t="s">
+      <c r="J35" t="s">
         <v>244</v>
       </c>
-      <c r="I35" t="s">
+      <c r="K35" t="s">
         <v>245</v>
       </c>
-      <c r="J35" t="s">
-        <v>246</v>
-      </c>
-      <c r="K35" t="s">
-        <v>247</v>
-      </c>
       <c r="L35" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="M35" t="s">
         <v>36</v>
       </c>
       <c r="N35" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="O35" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -3187,36 +3218,36 @@
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="H36" t="s">
+        <v>242</v>
+      </c>
+      <c r="I36" t="s">
+        <v>243</v>
+      </c>
+      <c r="J36" t="s">
         <v>244</v>
       </c>
-      <c r="I36" t="s">
+      <c r="K36" t="s">
         <v>245</v>
       </c>
-      <c r="J36" t="s">
-        <v>246</v>
-      </c>
-      <c r="K36" t="s">
-        <v>247</v>
-      </c>
       <c r="L36" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="M36" t="s">
         <v>36</v>
       </c>
       <c r="N36" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="O36" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -3226,36 +3257,54 @@
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="H37" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="I37" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="J37" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="K37" t="s">
-        <v>247</v>
-      </c>
-      <c r="L37" t="s">
-        <v>258</v>
+        <v>264</v>
+      </c>
+      <c r="L37">
+        <v>3320</v>
       </c>
       <c r="M37" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="N37" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="O37" t="s">
-        <v>260</v>
+        <v>266</v>
+      </c>
+      <c r="P37" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>268</v>
+      </c>
+      <c r="R37" t="s">
+        <v>269</v>
+      </c>
+      <c r="S37" t="s">
+        <v>24</v>
+      </c>
+      <c r="T37" t="s">
+        <v>270</v>
+      </c>
+      <c r="U37" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -3265,54 +3314,33 @@
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>262</v>
-      </c>
-      <c r="H38" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="I38" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="J38" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="K38" t="s">
-        <v>266</v>
-      </c>
-      <c r="L38">
-        <v>3320</v>
+        <v>276</v>
+      </c>
+      <c r="L38" t="s">
+        <v>277</v>
       </c>
       <c r="M38" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="N38" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="O38" t="s">
-        <v>268</v>
-      </c>
-      <c r="P38" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>270</v>
-      </c>
-      <c r="R38" t="s">
-        <v>271</v>
-      </c>
-      <c r="S38" t="s">
-        <v>24</v>
-      </c>
-      <c r="T38" t="s">
-        <v>272</v>
-      </c>
-      <c r="U38" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -3322,68 +3350,32 @@
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="I39" t="s">
+        <v>282</v>
+      </c>
+      <c r="J39" t="s">
+        <v>283</v>
+      </c>
+      <c r="K39" t="s">
         <v>276</v>
       </c>
-      <c r="J39" t="s">
-        <v>277</v>
-      </c>
-      <c r="K39" t="s">
-        <v>278</v>
-      </c>
       <c r="L39" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="M39" t="s">
         <v>36</v>
       </c>
       <c r="N39" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="O39" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>282</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F40" t="s">
-        <v>283</v>
-      </c>
-      <c r="I40" t="s">
-        <v>284</v>
-      </c>
-      <c r="J40" t="s">
-        <v>285</v>
-      </c>
-      <c r="K40" t="s">
-        <v>278</v>
-      </c>
-      <c r="L40" t="s">
         <v>286</v>
       </c>
-      <c r="M40" t="s">
-        <v>36</v>
-      </c>
-      <c r="N40" t="s">
-        <v>287</v>
-      </c>
-      <c r="O40" t="s">
-        <v>288</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E40">
+  <conditionalFormatting sqref="E2:E39">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>